<commit_message>
Added vimar and other data
</commit_message>
<xml_diff>
--- a/src/WebMarket/WebMarket/App_Data/Avr.xlsx
+++ b/src/WebMarket/WebMarket/App_Data/Avr.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="525" windowWidth="14805" windowHeight="7590"/>
+    <workbookView xWindow="240" yWindow="585" windowWidth="14805" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="Avr" sheetId="1" r:id="rId1"/>
@@ -17,8 +17,9 @@
     <definedName name="DisplayClassList">metadata!$B$2:$B$30</definedName>
     <definedName name="Producers" localSheetId="1">metadata!$A$2:$A$9</definedName>
     <definedName name="ProducersList">metadata!$A$2:$A$31</definedName>
+    <definedName name="Type">metadata!$D$2:$D$5</definedName>
   </definedNames>
-  <calcPr calcId="145621" refMode="R1C1"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -2031,15 +2032,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DisplayClass" refreshOnLoad="1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Producers" refreshOnLoad="1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Producers" refreshOnLoad="1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Availability" refreshOnLoad="1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Availability" refreshOnLoad="1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DisplayClass" refreshOnLoad="1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2335,8 +2336,8 @@
   <dimension ref="A1:AN265"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E100" sqref="E100"/>
+      <pane ySplit="1" topLeftCell="A244" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E253" sqref="E253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -5675,7 +5676,7 @@
       <c r="AJ50" s="7"/>
       <c r="AK50" s="7"/>
     </row>
-    <row r="51" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>99</v>
       </c>
@@ -5742,7 +5743,7 @@
       <c r="AJ51" s="1"/>
       <c r="AK51" s="1"/>
     </row>
-    <row r="52" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>101</v>
       </c>
@@ -5809,7 +5810,7 @@
       <c r="AJ52" s="1"/>
       <c r="AK52" s="1"/>
     </row>
-    <row r="53" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>102</v>
       </c>
@@ -5876,7 +5877,7 @@
       <c r="AJ53" s="1"/>
       <c r="AK53" s="1"/>
     </row>
-    <row r="54" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>103</v>
       </c>
@@ -5943,7 +5944,7 @@
       <c r="AJ54" s="1"/>
       <c r="AK54" s="1"/>
     </row>
-    <row r="55" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>104</v>
       </c>
@@ -6010,7 +6011,7 @@
       <c r="AJ55" s="1"/>
       <c r="AK55" s="1"/>
     </row>
-    <row r="56" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>105</v>
       </c>
@@ -6077,7 +6078,7 @@
       <c r="AJ56" s="1"/>
       <c r="AK56" s="1"/>
     </row>
-    <row r="57" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
         <v>107</v>
       </c>
@@ -6129,7 +6130,7 @@
       <c r="AJ57" s="1"/>
       <c r="AK57" s="1"/>
     </row>
-    <row r="58" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
         <v>108</v>
       </c>
@@ -6181,7 +6182,7 @@
       <c r="AJ58" s="1"/>
       <c r="AK58" s="1"/>
     </row>
-    <row r="59" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
         <v>109</v>
       </c>
@@ -6233,7 +6234,7 @@
       <c r="AJ59" s="1"/>
       <c r="AK59" s="1"/>
     </row>
-    <row r="60" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
         <v>261</v>
       </c>
@@ -6294,7 +6295,7 @@
       <c r="AJ60" s="1"/>
       <c r="AK60" s="1"/>
     </row>
-    <row r="61" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
         <v>262</v>
       </c>
@@ -6355,7 +6356,7 @@
       <c r="AJ61" s="1"/>
       <c r="AK61" s="1"/>
     </row>
-    <row r="62" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="s">
         <v>263</v>
       </c>
@@ -6414,7 +6415,7 @@
       <c r="AJ62" s="1"/>
       <c r="AK62" s="1"/>
     </row>
-    <row r="63" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A63" s="10" t="s">
         <v>110</v>
       </c>
@@ -6466,7 +6467,7 @@
       <c r="AJ63" s="1"/>
       <c r="AK63" s="1"/>
     </row>
-    <row r="64" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A64" s="10" t="s">
         <v>111</v>
       </c>
@@ -6518,7 +6519,7 @@
       <c r="AJ64" s="1"/>
       <c r="AK64" s="1"/>
     </row>
-    <row r="65" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A65" s="10" t="s">
         <v>112</v>
       </c>
@@ -6570,7 +6571,7 @@
       <c r="AJ65" s="1"/>
       <c r="AK65" s="1"/>
     </row>
-    <row r="66" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A66" s="10" t="s">
         <v>113</v>
       </c>
@@ -6622,7 +6623,7 @@
       <c r="AJ66" s="1"/>
       <c r="AK66" s="1"/>
     </row>
-    <row r="67" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="s">
         <v>114</v>
       </c>
@@ -6674,7 +6675,7 @@
       <c r="AJ67" s="1"/>
       <c r="AK67" s="1"/>
     </row>
-    <row r="68" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A68" s="10" t="s">
         <v>115</v>
       </c>
@@ -6720,7 +6721,7 @@
       <c r="AJ68" s="1"/>
       <c r="AK68" s="1"/>
     </row>
-    <row r="69" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A69" s="10" t="s">
         <v>116</v>
       </c>
@@ -6766,7 +6767,7 @@
       <c r="AJ69" s="1"/>
       <c r="AK69" s="1"/>
     </row>
-    <row r="70" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A70" s="10" t="s">
         <v>117</v>
       </c>
@@ -6815,7 +6816,7 @@
       <c r="AJ70" s="1"/>
       <c r="AK70" s="1"/>
     </row>
-    <row r="71" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A71" s="10" t="s">
         <v>118</v>
       </c>
@@ -6861,7 +6862,7 @@
       <c r="AJ71" s="1"/>
       <c r="AK71" s="1"/>
     </row>
-    <row r="72" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
         <v>119</v>
       </c>
@@ -6913,7 +6914,7 @@
       <c r="AJ72" s="1"/>
       <c r="AK72" s="1"/>
     </row>
-    <row r="73" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
         <v>120</v>
       </c>
@@ -6962,7 +6963,7 @@
       <c r="AJ73" s="1"/>
       <c r="AK73" s="1"/>
     </row>
-    <row r="74" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A74" s="10" t="s">
         <v>121</v>
       </c>
@@ -7011,7 +7012,7 @@
       <c r="AJ74" s="1"/>
       <c r="AK74" s="1"/>
     </row>
-    <row r="75" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A75" s="10" t="s">
         <v>122</v>
       </c>
@@ -7063,7 +7064,7 @@
       <c r="AJ75" s="1"/>
       <c r="AK75" s="1"/>
     </row>
-    <row r="76" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A76" s="10" t="s">
         <v>123</v>
       </c>
@@ -7115,7 +7116,7 @@
       <c r="AJ76" s="1"/>
       <c r="AK76" s="1"/>
     </row>
-    <row r="77" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A77" s="10" t="s">
         <v>124</v>
       </c>
@@ -7164,7 +7165,7 @@
       <c r="AJ77" s="1"/>
       <c r="AK77" s="1"/>
     </row>
-    <row r="78" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A78" s="10" t="s">
         <v>125</v>
       </c>
@@ -7213,7 +7214,7 @@
       <c r="AJ78" s="1"/>
       <c r="AK78" s="1"/>
     </row>
-    <row r="79" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A79" s="10" t="s">
         <v>126</v>
       </c>
@@ -7262,7 +7263,7 @@
       <c r="AJ79" s="1"/>
       <c r="AK79" s="1"/>
     </row>
-    <row r="80" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A80" s="10" t="s">
         <v>127</v>
       </c>
@@ -7311,7 +7312,7 @@
       <c r="AJ80" s="1"/>
       <c r="AK80" s="1"/>
     </row>
-    <row r="81" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A81" s="10" t="s">
         <v>128</v>
       </c>
@@ -7360,7 +7361,7 @@
       <c r="AJ81" s="1"/>
       <c r="AK81" s="1"/>
     </row>
-    <row r="82" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A82" s="10" t="s">
         <v>129</v>
       </c>
@@ -7412,7 +7413,7 @@
       <c r="AJ82" s="1"/>
       <c r="AK82" s="1"/>
     </row>
-    <row r="83" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A83" s="10" t="s">
         <v>130</v>
       </c>
@@ -7461,7 +7462,7 @@
       <c r="AJ83" s="1"/>
       <c r="AK83" s="1"/>
     </row>
-    <row r="84" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A84" s="10" t="s">
         <v>131</v>
       </c>
@@ -7510,7 +7511,7 @@
       <c r="AJ84" s="1"/>
       <c r="AK84" s="1"/>
     </row>
-    <row r="85" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A85" s="10" t="s">
         <v>132</v>
       </c>
@@ -7559,7 +7560,7 @@
       <c r="AJ85" s="1"/>
       <c r="AK85" s="1"/>
     </row>
-    <row r="86" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A86" s="10" t="s">
         <v>133</v>
       </c>
@@ -7608,7 +7609,7 @@
       <c r="AJ86" s="1"/>
       <c r="AK86" s="1"/>
     </row>
-    <row r="87" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A87" s="10" t="s">
         <v>134</v>
       </c>
@@ -7660,7 +7661,7 @@
       <c r="AJ87" s="1"/>
       <c r="AK87" s="1"/>
     </row>
-    <row r="88" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A88" s="10" t="s">
         <v>135</v>
       </c>
@@ -7709,7 +7710,7 @@
       <c r="AJ88" s="1"/>
       <c r="AK88" s="1"/>
     </row>
-    <row r="89" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A89" s="10" t="s">
         <v>136</v>
       </c>
@@ -7758,7 +7759,7 @@
       <c r="AJ89" s="1"/>
       <c r="AK89" s="1"/>
     </row>
-    <row r="90" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A90" s="10" t="s">
         <v>137</v>
       </c>
@@ -7810,7 +7811,7 @@
       <c r="AJ90" s="1"/>
       <c r="AK90" s="1"/>
     </row>
-    <row r="91" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A91" s="10" t="s">
         <v>138</v>
       </c>
@@ -7862,7 +7863,7 @@
       <c r="AJ91" s="1"/>
       <c r="AK91" s="1"/>
     </row>
-    <row r="92" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A92" s="10" t="s">
         <v>139</v>
       </c>
@@ -7914,7 +7915,7 @@
       <c r="AJ92" s="1"/>
       <c r="AK92" s="1"/>
     </row>
-    <row r="93" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A93" s="10" t="s">
         <v>140</v>
       </c>
@@ -7966,7 +7967,7 @@
       <c r="AJ93" s="1"/>
       <c r="AK93" s="1"/>
     </row>
-    <row r="94" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A94" s="10" t="s">
         <v>141</v>
       </c>
@@ -8015,7 +8016,7 @@
       <c r="AJ94" s="1"/>
       <c r="AK94" s="1"/>
     </row>
-    <row r="95" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A95" s="10" t="s">
         <v>142</v>
       </c>
@@ -8064,7 +8065,7 @@
       <c r="AJ95" s="1"/>
       <c r="AK95" s="1"/>
     </row>
-    <row r="96" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A96" s="10" t="s">
         <v>143</v>
       </c>
@@ -8113,7 +8114,7 @@
       <c r="AJ96" s="1"/>
       <c r="AK96" s="1"/>
     </row>
-    <row r="97" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A97" s="10" t="s">
         <v>144</v>
       </c>
@@ -8162,7 +8163,7 @@
       <c r="AJ97" s="1"/>
       <c r="AK97" s="1"/>
     </row>
-    <row r="98" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A98" s="10" t="s">
         <v>145</v>
       </c>
@@ -8211,7 +8212,7 @@
       <c r="AJ98" s="1"/>
       <c r="AK98" s="1"/>
     </row>
-    <row r="99" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A99" s="10" t="s">
         <v>146</v>
       </c>
@@ -8266,7 +8267,7 @@
       <c r="AJ99" s="1"/>
       <c r="AK99" s="1"/>
     </row>
-    <row r="100" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A100" s="10" t="s">
         <v>264</v>
       </c>
@@ -8312,7 +8313,7 @@
       <c r="AJ100" s="1"/>
       <c r="AK100" s="1"/>
     </row>
-    <row r="101" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A101" s="10" t="s">
         <v>147</v>
       </c>
@@ -8367,7 +8368,7 @@
       <c r="AJ101" s="1"/>
       <c r="AK101" s="1"/>
     </row>
-    <row r="102" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A102" s="10" t="s">
         <v>149</v>
       </c>
@@ -8422,7 +8423,7 @@
       <c r="AJ102" s="1"/>
       <c r="AK102" s="1"/>
     </row>
-    <row r="103" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A103" s="11" t="s">
         <v>150</v>
       </c>
@@ -8471,7 +8472,7 @@
       <c r="AJ103" s="1"/>
       <c r="AK103" s="1"/>
     </row>
-    <row r="104" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A104" s="11" t="s">
         <v>151</v>
       </c>
@@ -8520,7 +8521,7 @@
       <c r="AJ104" s="1"/>
       <c r="AK104" s="1"/>
     </row>
-    <row r="105" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A105" s="11" t="s">
         <v>152</v>
       </c>
@@ -8569,7 +8570,7 @@
       <c r="AJ105" s="1"/>
       <c r="AK105" s="1"/>
     </row>
-    <row r="106" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A106" s="11" t="s">
         <v>153</v>
       </c>
@@ -8618,7 +8619,7 @@
       <c r="AJ106" s="1"/>
       <c r="AK106" s="1"/>
     </row>
-    <row r="107" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A107" s="11" t="s">
         <v>154</v>
       </c>
@@ -8670,7 +8671,7 @@
       <c r="AJ107" s="1"/>
       <c r="AK107" s="1"/>
     </row>
-    <row r="108" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A108" s="11" t="s">
         <v>155</v>
       </c>
@@ -8722,7 +8723,7 @@
       <c r="AJ108" s="1"/>
       <c r="AK108" s="1"/>
     </row>
-    <row r="109" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A109" s="11" t="s">
         <v>156</v>
       </c>
@@ -8771,7 +8772,7 @@
       <c r="AJ109" s="1"/>
       <c r="AK109" s="1"/>
     </row>
-    <row r="110" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A110" s="11" t="s">
         <v>157</v>
       </c>
@@ -8823,7 +8824,7 @@
       <c r="AJ110" s="1"/>
       <c r="AK110" s="1"/>
     </row>
-    <row r="111" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A111" s="11" t="s">
         <v>158</v>
       </c>
@@ -8878,7 +8879,7 @@
       <c r="AJ111" s="1"/>
       <c r="AK111" s="1"/>
     </row>
-    <row r="112" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A112" s="11" t="s">
         <v>160</v>
       </c>
@@ -8933,7 +8934,7 @@
       <c r="AJ112" s="1"/>
       <c r="AK112" s="1"/>
     </row>
-    <row r="113" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A113" s="12" t="s">
         <v>161</v>
       </c>
@@ -8988,7 +8989,7 @@
       <c r="AJ113" s="1"/>
       <c r="AK113" s="1"/>
     </row>
-    <row r="114" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A114" s="12" t="s">
         <v>163</v>
       </c>
@@ -9037,7 +9038,7 @@
       <c r="AJ114" s="1"/>
       <c r="AK114" s="1"/>
     </row>
-    <row r="115" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A115" s="12" t="s">
         <v>164</v>
       </c>
@@ -9092,7 +9093,7 @@
       <c r="AJ115" s="1"/>
       <c r="AK115" s="1"/>
     </row>
-    <row r="116" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A116" s="12" t="s">
         <v>166</v>
       </c>
@@ -9141,7 +9142,7 @@
       <c r="AJ116" s="1"/>
       <c r="AK116" s="1"/>
     </row>
-    <row r="117" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A117" s="12" t="s">
         <v>167</v>
       </c>
@@ -9196,7 +9197,7 @@
       <c r="AJ117" s="1"/>
       <c r="AK117" s="1"/>
     </row>
-    <row r="118" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A118" s="12" t="s">
         <v>169</v>
       </c>
@@ -9251,7 +9252,7 @@
       <c r="AJ118" s="1"/>
       <c r="AK118" s="1"/>
     </row>
-    <row r="119" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A119" s="12" t="s">
         <v>171</v>
       </c>
@@ -9306,7 +9307,7 @@
       <c r="AJ119" s="1"/>
       <c r="AK119" s="1"/>
     </row>
-    <row r="120" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A120" s="12" t="s">
         <v>172</v>
       </c>
@@ -9355,7 +9356,7 @@
       <c r="AJ120" s="1"/>
       <c r="AK120" s="1"/>
     </row>
-    <row r="121" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A121" s="12" t="s">
         <v>173</v>
       </c>
@@ -9404,7 +9405,7 @@
       <c r="AJ121" s="1"/>
       <c r="AK121" s="1"/>
     </row>
-    <row r="122" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A122" s="12" t="s">
         <v>174</v>
       </c>
@@ -9453,7 +9454,7 @@
       <c r="AJ122" s="1"/>
       <c r="AK122" s="1"/>
     </row>
-    <row r="123" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A123" s="12" t="s">
         <v>175</v>
       </c>
@@ -9502,7 +9503,7 @@
       <c r="AJ123" s="1"/>
       <c r="AK123" s="1"/>
     </row>
-    <row r="124" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A124" s="12" t="s">
         <v>176</v>
       </c>
@@ -9551,7 +9552,7 @@
       <c r="AJ124" s="1"/>
       <c r="AK124" s="1"/>
     </row>
-    <row r="125" spans="1:37" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:37" s="6" customFormat="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A125" s="13" t="s">
         <v>177</v>
       </c>
@@ -9603,7 +9604,7 @@
       <c r="AJ125" s="7"/>
       <c r="AK125" s="7"/>
     </row>
-    <row r="126" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
         <v>293</v>
       </c>
@@ -9656,7 +9657,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="127" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
         <v>294</v>
       </c>
@@ -9709,7 +9710,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="128" spans="1:37" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:37" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
         <v>295</v>
       </c>
@@ -9762,7 +9763,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="129" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
         <v>296</v>
       </c>
@@ -9815,7 +9816,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="130" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
         <v>297</v>
       </c>
@@ -9868,7 +9869,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="131" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
         <v>298</v>
       </c>
@@ -9921,7 +9922,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="132" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
         <v>310</v>
       </c>
@@ -9974,7 +9975,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="133" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
         <v>299</v>
       </c>
@@ -10027,7 +10028,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="134" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
         <v>300</v>
       </c>
@@ -10080,7 +10081,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="135" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
         <v>301</v>
       </c>
@@ -10133,7 +10134,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="136" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
         <v>302</v>
       </c>
@@ -10186,7 +10187,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="137" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
         <v>303</v>
       </c>
@@ -10239,7 +10240,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="138" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
         <v>304</v>
       </c>
@@ -10292,7 +10293,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="139" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
         <v>305</v>
       </c>
@@ -10345,7 +10346,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="140" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
         <v>306</v>
       </c>
@@ -10398,7 +10399,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="141" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
         <v>307</v>
       </c>
@@ -10451,7 +10452,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="142" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
         <v>308</v>
       </c>
@@ -10504,7 +10505,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="143" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
         <v>309</v>
       </c>
@@ -10557,7 +10558,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="144" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
         <v>313</v>
       </c>
@@ -10607,7 +10608,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="145" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
         <v>316</v>
       </c>
@@ -10660,7 +10661,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="146" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
         <v>315</v>
       </c>
@@ -10713,7 +10714,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="147" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
         <v>317</v>
       </c>
@@ -10766,7 +10767,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="148" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
         <v>318</v>
       </c>
@@ -10819,7 +10820,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="149" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
         <v>319</v>
       </c>
@@ -10872,7 +10873,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="150" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
         <v>320</v>
       </c>
@@ -10925,7 +10926,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="151" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
         <v>321</v>
       </c>
@@ -10978,7 +10979,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="152" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
         <v>322</v>
       </c>
@@ -11031,7 +11032,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="153" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
         <v>323</v>
       </c>
@@ -11084,7 +11085,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="154" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
         <v>324</v>
       </c>
@@ -11137,7 +11138,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="155" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
         <v>325</v>
       </c>
@@ -11190,7 +11191,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="156" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
         <v>326</v>
       </c>
@@ -11243,7 +11244,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="157" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
         <v>328</v>
       </c>
@@ -11296,7 +11297,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="158" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
         <v>342</v>
       </c>
@@ -11349,7 +11350,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="159" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
         <v>330</v>
       </c>
@@ -11402,7 +11403,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="160" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
         <v>331</v>
       </c>
@@ -11455,7 +11456,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="161" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
         <v>332</v>
       </c>
@@ -11508,7 +11509,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="162" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
         <v>333</v>
       </c>
@@ -11561,7 +11562,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="163" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
         <v>334</v>
       </c>
@@ -11614,7 +11615,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="164" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
         <v>335</v>
       </c>
@@ -11667,7 +11668,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="165" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
         <v>336</v>
       </c>
@@ -11720,7 +11721,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="166" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
         <v>337</v>
       </c>
@@ -11773,7 +11774,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="167" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
         <v>356</v>
       </c>
@@ -11826,7 +11827,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="168" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
         <v>338</v>
       </c>
@@ -11879,7 +11880,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="169" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
         <v>339</v>
       </c>
@@ -11932,7 +11933,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="170" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
         <v>340</v>
       </c>
@@ -11985,7 +11986,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="171" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A171" s="3" t="s">
         <v>341</v>
       </c>
@@ -12038,7 +12039,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="172" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A172" s="3" t="s">
         <v>355</v>
       </c>
@@ -12082,7 +12083,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="173" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="s">
         <v>343</v>
       </c>
@@ -12135,7 +12136,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="174" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A174" s="3" t="s">
         <v>344</v>
       </c>
@@ -12188,7 +12189,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="175" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A175" s="3" t="s">
         <v>345</v>
       </c>
@@ -12241,7 +12242,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="176" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A176" s="3" t="s">
         <v>346</v>
       </c>
@@ -12294,7 +12295,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="177" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
         <v>347</v>
       </c>
@@ -12347,7 +12348,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="178" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A178" s="3" t="s">
         <v>348</v>
       </c>
@@ -12400,7 +12401,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="179" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A179" s="3" t="s">
         <v>349</v>
       </c>
@@ -12453,7 +12454,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="180" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A180" s="3" t="s">
         <v>350</v>
       </c>
@@ -12506,7 +12507,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="181" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A181" s="3" t="s">
         <v>358</v>
       </c>
@@ -12553,7 +12554,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="182" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A182" s="3" t="s">
         <v>351</v>
       </c>
@@ -12606,7 +12607,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="183" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A183" s="3" t="s">
         <v>352</v>
       </c>
@@ -12659,7 +12660,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="184" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A184" s="3" t="s">
         <v>353</v>
       </c>
@@ -12712,7 +12713,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="185" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A185" s="3" t="s">
         <v>354</v>
       </c>
@@ -12765,7 +12766,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="186" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A186" s="3" t="s">
         <v>371</v>
       </c>
@@ -12812,7 +12813,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="187" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A187" s="3" t="s">
         <v>359</v>
       </c>
@@ -12865,7 +12866,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="188" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A188" s="3" t="s">
         <v>360</v>
       </c>
@@ -12918,7 +12919,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="189" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A189" s="3" t="s">
         <v>361</v>
       </c>
@@ -12971,7 +12972,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="190" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A190" s="3" t="s">
         <v>362</v>
       </c>
@@ -13024,7 +13025,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="191" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A191" s="3" t="s">
         <v>363</v>
       </c>
@@ -13077,7 +13078,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="192" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A192" s="3" t="s">
         <v>364</v>
       </c>
@@ -13130,7 +13131,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="193" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A193" s="3" t="s">
         <v>365</v>
       </c>
@@ -13183,7 +13184,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="194" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A194" s="3" t="s">
         <v>366</v>
       </c>
@@ -13236,7 +13237,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="195" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A195" s="3" t="s">
         <v>372</v>
       </c>
@@ -13283,7 +13284,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="196" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A196" s="3" t="s">
         <v>367</v>
       </c>
@@ -13336,7 +13337,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="197" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A197" s="3" t="s">
         <v>368</v>
       </c>
@@ -13389,7 +13390,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="198" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A198" s="3" t="s">
         <v>369</v>
       </c>
@@ -13442,7 +13443,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="199" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A199" s="3" t="s">
         <v>370</v>
       </c>
@@ -13495,7 +13496,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="200" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A200" s="3" t="s">
         <v>373</v>
       </c>
@@ -13548,7 +13549,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="201" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A201" s="3" t="s">
         <v>374</v>
       </c>
@@ -13601,7 +13602,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="202" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A202" s="3" t="s">
         <v>375</v>
       </c>
@@ -13654,7 +13655,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="203" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A203" s="3" t="s">
         <v>376</v>
       </c>
@@ -13707,7 +13708,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="204" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A204" s="3" t="s">
         <v>377</v>
       </c>
@@ -13760,7 +13761,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="205" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A205" s="3" t="s">
         <v>378</v>
       </c>
@@ -13813,7 +13814,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="206" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A206" s="3" t="s">
         <v>379</v>
       </c>
@@ -13866,7 +13867,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="207" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A207" s="3" t="s">
         <v>380</v>
       </c>
@@ -13919,7 +13920,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="208" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A208" s="3" t="s">
         <v>381</v>
       </c>
@@ -13972,7 +13973,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="209" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A209" s="3" t="s">
         <v>382</v>
       </c>
@@ -14025,7 +14026,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="210" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A210" s="3" t="s">
         <v>383</v>
       </c>
@@ -14078,7 +14079,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="211" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A211" s="3" t="s">
         <v>384</v>
       </c>
@@ -14131,7 +14132,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="212" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A212" s="3" t="s">
         <v>385</v>
       </c>
@@ -14184,7 +14185,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="213" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A213" s="3" t="s">
         <v>386</v>
       </c>
@@ -14237,7 +14238,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="214" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A214" s="3" t="s">
         <v>387</v>
       </c>
@@ -14290,7 +14291,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="215" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A215" s="3" t="s">
         <v>388</v>
       </c>
@@ -14343,7 +14344,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="216" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A216" s="3" t="s">
         <v>389</v>
       </c>
@@ -14396,7 +14397,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="217" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A217" s="3" t="s">
         <v>398</v>
       </c>
@@ -14449,7 +14450,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="218" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A218" s="3" t="s">
         <v>390</v>
       </c>
@@ -14502,7 +14503,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="219" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A219" s="3" t="s">
         <v>391</v>
       </c>
@@ -14555,7 +14556,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="220" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A220" s="3" t="s">
         <v>392</v>
       </c>
@@ -14608,7 +14609,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="221" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A221" s="3" t="s">
         <v>393</v>
       </c>
@@ -14661,7 +14662,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="222" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A222" s="3" t="s">
         <v>394</v>
       </c>
@@ -14714,7 +14715,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="223" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A223" s="3" t="s">
         <v>395</v>
       </c>
@@ -14767,7 +14768,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="224" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A224" s="3" t="s">
         <v>396</v>
       </c>
@@ -14820,7 +14821,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="225" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A225" s="3" t="s">
         <v>397</v>
       </c>
@@ -14873,7 +14874,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="226" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A226" s="3" t="s">
         <v>399</v>
       </c>
@@ -14926,7 +14927,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="227" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A227" s="3" t="s">
         <v>400</v>
       </c>
@@ -14979,7 +14980,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="228" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A228" s="3" t="s">
         <v>401</v>
       </c>
@@ -15032,7 +15033,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="229" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A229" s="3" t="s">
         <v>402</v>
       </c>
@@ -15085,7 +15086,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="230" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A230" s="3" t="s">
         <v>403</v>
       </c>
@@ -15138,7 +15139,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="231" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A231" s="3" t="s">
         <v>404</v>
       </c>
@@ -15191,7 +15192,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="232" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A232" s="3" t="s">
         <v>405</v>
       </c>
@@ -15244,7 +15245,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="233" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A233" s="3" t="s">
         <v>406</v>
       </c>
@@ -15297,7 +15298,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="234" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A234" s="3" t="s">
         <v>407</v>
       </c>
@@ -15350,7 +15351,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="235" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A235" s="3" t="s">
         <v>408</v>
       </c>
@@ -15403,7 +15404,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="236" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A236" s="3" t="s">
         <v>410</v>
       </c>
@@ -15456,7 +15457,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="237" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A237" s="3" t="s">
         <v>411</v>
       </c>
@@ -15509,7 +15510,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="238" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A238" s="3" t="s">
         <v>412</v>
       </c>
@@ -15562,7 +15563,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="239" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A239" s="3" t="s">
         <v>413</v>
       </c>
@@ -15615,7 +15616,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="240" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A240" s="3" t="s">
         <v>414</v>
       </c>
@@ -15668,7 +15669,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="241" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A241" s="3" t="s">
         <v>415</v>
       </c>
@@ -15721,7 +15722,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="242" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A242" s="3" t="s">
         <v>416</v>
       </c>
@@ -15774,7 +15775,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="243" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A243" s="4" t="s">
         <v>417</v>
       </c>
@@ -15827,7 +15828,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="244" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A244" s="4" t="s">
         <v>418</v>
       </c>
@@ -15880,7 +15881,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="245" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A245" s="4" t="s">
         <v>419</v>
       </c>
@@ -15933,7 +15934,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="246" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A246" s="4" t="s">
         <v>426</v>
       </c>
@@ -15983,7 +15984,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="247" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A247" s="4" t="s">
         <v>420</v>
       </c>
@@ -16036,7 +16037,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="248" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A248" s="4" t="s">
         <v>421</v>
       </c>
@@ -16089,7 +16090,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="249" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A249" s="4" t="s">
         <v>422</v>
       </c>
@@ -16142,7 +16143,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="250" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A250" s="4" t="s">
         <v>427</v>
       </c>
@@ -16192,7 +16193,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="251" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A251" s="4" t="s">
         <v>423</v>
       </c>
@@ -16245,7 +16246,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="252" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A252" s="4" t="s">
         <v>424</v>
       </c>
@@ -16298,7 +16299,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="253" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A253" s="4" t="s">
         <v>425</v>
       </c>
@@ -16351,7 +16352,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="254" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A254" s="4" t="s">
         <v>428</v>
       </c>
@@ -16401,7 +16402,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="255" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A255" s="5" t="s">
         <v>429</v>
       </c>
@@ -16424,7 +16425,7 @@
         <v>0</v>
       </c>
       <c r="I255">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="J255">
         <v>5</v>
@@ -16454,7 +16455,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="256" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A256" s="5" t="s">
         <v>430</v>
       </c>
@@ -16477,7 +16478,7 @@
         <v>0</v>
       </c>
       <c r="I256">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="J256">
         <v>5</v>
@@ -16507,7 +16508,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="257" spans="1:31" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:31" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A257" s="5" t="s">
         <v>431</v>
       </c>
@@ -16530,7 +16531,7 @@
         <v>0</v>
       </c>
       <c r="I257">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="J257">
         <v>5</v>
@@ -16560,7 +16561,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="258" spans="1:31" s="6" customFormat="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A258" s="21" t="s">
         <v>432</v>
       </c>
@@ -16583,7 +16584,7 @@
         <v>0</v>
       </c>
       <c r="I258" s="6">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="J258" s="6">
         <v>5</v>
@@ -16991,7 +16992,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">
       <formula1>AvailabilityList</formula1>
     </dataValidation>
@@ -17000,6 +17001,9 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576">
       <formula1>ProducersList</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576">
+      <formula1>Type</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17013,7 +17017,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>